<commit_message>
working CI with time_filter and first_treshold_filter
</commit_message>
<xml_diff>
--- a/processed_CI_test_data/pivots_CI_test.xlsx
+++ b/processed_CI_test_data/pivots_CI_test.xlsx
@@ -511,34 +511,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="C4" t="n">
-        <v>27.73722627737226</v>
+        <v>30.41362530413625</v>
       </c>
       <c r="D4" t="n">
-        <v>9.238095238093175</v>
+        <v>9.272727272725254</v>
       </c>
       <c r="E4" t="n">
-        <v>8.878548434686927</v>
+        <v>8.819115682298605</v>
       </c>
       <c r="F4" t="n">
-        <v>-8.487615699492618</v>
+        <v>-8.541584193803192</v>
       </c>
       <c r="G4" t="n">
-        <v>-31557315.47</v>
+        <v>-34640745.33</v>
       </c>
       <c r="H4" t="n">
-        <v>28.86891091284728</v>
+        <v>31.6896597822806</v>
       </c>
       <c r="I4" t="n">
-        <v>3718042.45</v>
+        <v>4055541.05</v>
       </c>
       <c r="J4" t="n">
-        <v>29.99938878758648</v>
+        <v>32.72252921775185</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1178187179303817</v>
+        <v>0.1170743011261877</v>
       </c>
     </row>
     <row r="5">
@@ -566,7 +566,7 @@
         <v>-62164145.07</v>
       </c>
       <c r="H5" t="n">
-        <v>56.86830895692614</v>
+        <v>56.86830895692613</v>
       </c>
       <c r="I5" t="n">
         <v>2740466.74</v>
@@ -585,34 +585,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C6" t="n">
-        <v>9.48905109489051</v>
+        <v>6.81265206812652</v>
       </c>
       <c r="D6" t="n">
-        <v>9.187499999998433</v>
+        <v>9.071428571426937</v>
       </c>
       <c r="E6" t="n">
-        <v>8.714910683939751</v>
+        <v>8.880237208408307</v>
       </c>
       <c r="F6" t="n">
-        <v>-8.864049094165761</v>
+        <v>-8.77210559852967</v>
       </c>
       <c r="G6" t="n">
-        <v>-11844296.9</v>
+        <v>-8760867.040000001</v>
       </c>
       <c r="H6" t="n">
-        <v>10.8352674154578</v>
+        <v>8.014518546024476</v>
       </c>
       <c r="I6" t="n">
-        <v>1336217.43</v>
+        <v>998718.83</v>
       </c>
       <c r="J6" t="n">
-        <v>10.78140089210644</v>
+        <v>8.058260461941064</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1128152596377418</v>
+        <v>0.113997715687282</v>
       </c>
     </row>
     <row r="7">
@@ -622,34 +622,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="C7" t="n">
-        <v>20.92457420924574</v>
+        <v>24.45255474452555</v>
       </c>
       <c r="D7" t="n">
-        <v>11.96774193548222</v>
+        <v>11.79411764705722</v>
       </c>
       <c r="E7" t="n">
-        <v>9.037038767169918</v>
+        <v>8.935403436059238</v>
       </c>
       <c r="F7" t="n">
-        <v>2.520415041573554</v>
+        <v>1.935693512809962</v>
       </c>
       <c r="G7" t="n">
-        <v>5804467.6</v>
+        <v>5178903.55</v>
       </c>
       <c r="H7" t="n">
-        <v>-5.309978226766717</v>
+        <v>-4.737706708712587</v>
       </c>
       <c r="I7" t="n">
-        <v>2302980.86</v>
+        <v>2675477.04</v>
       </c>
       <c r="J7" t="n">
-        <v>18.58182608687274</v>
+        <v>21.58734791078597</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3967600508270561</v>
+        <v>0.5166107100025062</v>
       </c>
     </row>
     <row r="8">
@@ -677,7 +677,7 @@
         <v>-6014092.609999999</v>
       </c>
       <c r="H8" t="n">
-        <v>5.501745037367185</v>
+        <v>5.501745037367184</v>
       </c>
       <c r="I8" t="n">
         <v>1168909.05</v>
@@ -696,34 +696,34 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C9" t="n">
-        <v>10.34063260340633</v>
+        <v>6.81265206812652</v>
       </c>
       <c r="D9" t="n">
-        <v>10.91666666666317</v>
+        <v>11.04761904761521</v>
       </c>
       <c r="E9" t="n">
-        <v>9.49692489835707</v>
+        <v>10.04010317147585</v>
       </c>
       <c r="F9" t="n">
-        <v>-3.138177079501172</v>
+        <v>-3.858273010158841</v>
       </c>
       <c r="G9" t="n">
-        <v>-3537073.31</v>
+        <v>-2911509.26</v>
       </c>
       <c r="H9" t="n">
-        <v>3.235745904168313</v>
+        <v>2.663474386114185</v>
       </c>
       <c r="I9" t="n">
-        <v>1127110.81</v>
+        <v>754614.63</v>
       </c>
       <c r="J9" t="n">
-        <v>9.094203697400365</v>
+        <v>6.088681873487141</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3186563328538984</v>
+        <v>0.2591833178644948</v>
       </c>
     </row>
     <row r="10">
@@ -799,34 +799,34 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="C13" t="n">
-        <v>26.52068126520681</v>
+        <v>27.85888077858881</v>
       </c>
       <c r="D13" t="n">
-        <v>9.772727272726833</v>
+        <v>9.749999999999385</v>
       </c>
       <c r="E13" t="n">
-        <v>12.09168907504161</v>
+        <v>12.00406084482989</v>
       </c>
       <c r="F13" t="n">
-        <v>-3.404278122799059</v>
+        <v>-4.021814159756309</v>
       </c>
       <c r="G13" t="n">
-        <v>-6638549.013183</v>
+        <v>-8438455.526552001</v>
       </c>
       <c r="H13" t="n">
-        <v>6.871913952450208</v>
+        <v>8.735092586480651</v>
       </c>
       <c r="I13" t="n">
-        <v>1950060.71</v>
+        <v>2098171.42</v>
       </c>
       <c r="J13" t="n">
-        <v>25.9855159511088</v>
+        <v>27.95916384704279</v>
       </c>
       <c r="K13" t="n">
-        <v>0.2937480323075901</v>
+        <v>0.248644009961065</v>
       </c>
     </row>
     <row r="14">
@@ -860,7 +860,7 @@
         <v>1314515.19</v>
       </c>
       <c r="J14" t="n">
-        <v>17.51656000377538</v>
+        <v>17.51656000377537</v>
       </c>
       <c r="K14" t="n">
         <v>0.02367357443575295</v>
@@ -873,34 +873,34 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C15" t="n">
-        <v>12.04379562043796</v>
+        <v>10.70559610705596</v>
       </c>
       <c r="D15" t="n">
-        <v>11.2285714285689</v>
+        <v>11.7037037037009</v>
       </c>
       <c r="E15" t="n">
-        <v>11.97877220222749</v>
+        <v>12.18693181601338</v>
       </c>
       <c r="F15" t="n">
-        <v>-7.884856609133799</v>
+        <v>-7.147936317087676</v>
       </c>
       <c r="G15" t="n">
-        <v>-7930868.6898764</v>
+        <v>-6130962.1765074</v>
       </c>
       <c r="H15" t="n">
-        <v>8.209662547762193</v>
+        <v>6.34648391373175</v>
       </c>
       <c r="I15" t="n">
-        <v>1005835.5</v>
+        <v>857724.79</v>
       </c>
       <c r="J15" t="n">
-        <v>13.40325165027375</v>
+        <v>11.42960375433975</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1268253881550113</v>
+        <v>0.1399005189245217</v>
       </c>
     </row>
     <row r="16">
@@ -910,34 +910,34 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="C16" t="n">
-        <v>24.57420924574209</v>
+        <v>27.12895377128954</v>
       </c>
       <c r="D16" t="n">
-        <v>12.78571428571295</v>
+        <v>12.05555555555461</v>
       </c>
       <c r="E16" t="n">
-        <v>13.67759435802634</v>
+        <v>13.65524693533521</v>
       </c>
       <c r="F16" t="n">
-        <v>2.248195909627059</v>
+        <v>0.8208220310096294</v>
       </c>
       <c r="G16" t="n">
-        <v>3985920.412839</v>
+        <v>1585319.55795553</v>
       </c>
       <c r="H16" t="n">
-        <v>-4.126037488606451</v>
+        <v>-1.641048302539133</v>
       </c>
       <c r="I16" t="n">
-        <v>1772941.76</v>
+        <v>1931380.37</v>
       </c>
       <c r="J16" t="n">
-        <v>23.62531902140981</v>
+        <v>25.73659125325048</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4448010939428693</v>
+        <v>1.218290886722397</v>
       </c>
     </row>
     <row r="17">
@@ -971,7 +971,7 @@
         <v>407412.46</v>
       </c>
       <c r="J17" t="n">
-        <v>5.428970966760557</v>
+        <v>5.428970966760556</v>
       </c>
       <c r="K17" t="n">
         <v>0.02163979095853083</v>
@@ -984,34 +984,34 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C18" t="n">
-        <v>13.62530413625304</v>
+        <v>11.0705596107056</v>
       </c>
       <c r="D18" t="n">
-        <v>14.63157894736813</v>
+        <v>15.99999999999951</v>
       </c>
       <c r="E18" t="n">
-        <v>13.19444469477684</v>
+        <v>13.15019046450818</v>
       </c>
       <c r="F18" t="n">
-        <v>-11.07284479295192</v>
+        <v>-10.35096406431735</v>
       </c>
       <c r="G18" t="n">
-        <v>-11666885.53172747</v>
+        <v>-9266284.676844001</v>
       </c>
       <c r="H18" t="n">
-        <v>12.0770116041783</v>
+        <v>9.592022418110979</v>
       </c>
       <c r="I18" t="n">
-        <v>1053648.43</v>
+        <v>895209.8199999999</v>
       </c>
       <c r="J18" t="n">
-        <v>14.04038240667171</v>
+        <v>11.92911017483104</v>
       </c>
       <c r="K18" t="n">
-        <v>0.09031102834896763</v>
+        <v>0.09660935868256737</v>
       </c>
     </row>
     <row r="19">
@@ -1087,34 +1087,34 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="C22" t="n">
-        <v>27.12895377128954</v>
+        <v>28.83211678832117</v>
       </c>
       <c r="D22" t="n">
         <v>13.38888888888646</v>
       </c>
       <c r="E22" t="n">
-        <v>9.940902532305131</v>
+        <v>9.910696426606913</v>
       </c>
       <c r="F22" t="n">
-        <v>-12.22176932205215</v>
+        <v>-11.7803804837042</v>
       </c>
       <c r="G22" t="n">
-        <v>-8613794</v>
+        <v>-8673295</v>
       </c>
       <c r="H22" t="n">
-        <v>19.65906926116899</v>
+        <v>19.79486706177913</v>
       </c>
       <c r="I22" t="n">
-        <v>704791.08</v>
+        <v>736249.14</v>
       </c>
       <c r="J22" t="n">
-        <v>28.42338840856644</v>
+        <v>29.69205466064214</v>
       </c>
       <c r="K22" t="n">
-        <v>0.08182121374158703</v>
+        <v>0.08488690169076459</v>
       </c>
     </row>
     <row r="23">
@@ -1148,7 +1148,7 @@
         <v>868403.98</v>
       </c>
       <c r="J23" t="n">
-        <v>35.02170262864985</v>
+        <v>35.02170262864984</v>
       </c>
       <c r="K23" t="n">
         <v>0.03041387547207134</v>
@@ -1161,34 +1161,34 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C24" t="n">
-        <v>9.367396593673966</v>
+        <v>7.664233576642336</v>
       </c>
       <c r="D24" t="n">
         <v>12.1666666666643</v>
       </c>
       <c r="E24" t="n">
-        <v>10.82243276997216</v>
+        <v>11.11948195726272</v>
       </c>
       <c r="F24" t="n">
-        <v>-11.88430391802303</v>
+        <v>-13.16308069710867</v>
       </c>
       <c r="G24" t="n">
-        <v>-3295324</v>
+        <v>-3235823</v>
       </c>
       <c r="H24" t="n">
-        <v>7.520844212665459</v>
+        <v>7.38504641205532</v>
       </c>
       <c r="I24" t="n">
-        <v>277283.72</v>
+        <v>245825.66</v>
       </c>
       <c r="J24" t="n">
-        <v>11.18252358263697</v>
+        <v>9.913857330561269</v>
       </c>
       <c r="K24" t="n">
-        <v>0.08414460004539766</v>
+        <v>0.07597005769475031</v>
       </c>
     </row>
     <row r="25">
@@ -1198,34 +1198,34 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="C25" t="n">
-        <v>18.73479318734793</v>
+        <v>21.53284671532846</v>
       </c>
       <c r="D25" t="n">
         <v>13.11111111110734</v>
       </c>
       <c r="E25" t="n">
-        <v>9.938386263427697</v>
+        <v>9.946360747452687</v>
       </c>
       <c r="F25" t="n">
-        <v>-3.227603221084285</v>
+        <v>-2.643305400783881</v>
       </c>
       <c r="G25" t="n">
-        <v>-910511</v>
+        <v>-828485</v>
       </c>
       <c r="H25" t="n">
-        <v>2.078038877184228</v>
+        <v>1.890832773205349</v>
       </c>
       <c r="I25" t="n">
-        <v>282101.28</v>
+        <v>313427.65</v>
       </c>
       <c r="J25" t="n">
-        <v>11.37681006404587</v>
+        <v>12.64016541459949</v>
       </c>
       <c r="K25" t="n">
-        <v>0.3098274265769442</v>
+        <v>0.3783142120859159</v>
       </c>
     </row>
     <row r="26">
@@ -1272,34 +1272,34 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C27" t="n">
-        <v>9.732360097323602</v>
+        <v>6.934306569343065</v>
       </c>
       <c r="D27" t="n">
         <v>15.68750000000024</v>
       </c>
       <c r="E27" t="n">
-        <v>10.7506861222591</v>
+        <v>11.03237192774904</v>
       </c>
       <c r="F27" t="n">
-        <v>-1.646691407231437</v>
+        <v>-2.634629225882044</v>
       </c>
       <c r="G27" t="n">
-        <v>-274287</v>
+        <v>-356313</v>
       </c>
       <c r="H27" t="n">
-        <v>0.6259990812919672</v>
+        <v>0.8132051852708466</v>
       </c>
       <c r="I27" t="n">
-        <v>166568.55</v>
+        <v>135242.18</v>
       </c>
       <c r="J27" t="n">
-        <v>6.717512079326713</v>
+        <v>5.454156728773094</v>
       </c>
       <c r="K27" t="n">
-        <v>0.6072783252578503</v>
+        <v>0.3795600497315562</v>
       </c>
     </row>
     <row r="28">
@@ -1375,34 +1375,34 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C31" t="n">
-        <v>25.98039215686275</v>
+        <v>27.94117647058824</v>
       </c>
       <c r="D31" t="n">
-        <v>20.34042553191913</v>
+        <v>20.39583333333752</v>
       </c>
       <c r="E31" t="n">
-        <v>27.05374731865533</v>
+        <v>26.9955004944855</v>
       </c>
       <c r="F31" t="n">
-        <v>-42.97524070414862</v>
+        <v>-41.87690390271638</v>
       </c>
       <c r="G31" t="n">
-        <v>-163151653.76</v>
+        <v>-166101987.18</v>
       </c>
       <c r="H31" t="n">
-        <v>41.21563991887894</v>
+        <v>41.96095801450934</v>
       </c>
       <c r="I31" t="n">
-        <v>3796410.47</v>
+        <v>3966434.28</v>
       </c>
       <c r="J31" t="n">
-        <v>29.16568814493266</v>
+        <v>30.47188552766016</v>
       </c>
       <c r="K31" t="n">
-        <v>0.02326921230957678</v>
+        <v>0.02387951130110013</v>
       </c>
     </row>
     <row r="32">
@@ -1449,34 +1449,34 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C33" t="n">
-        <v>7.475490196078431</v>
+        <v>5.514705882352941</v>
       </c>
       <c r="D33" t="n">
-        <v>20.6666666666706</v>
+        <v>20.20000000000436</v>
       </c>
       <c r="E33" t="n">
-        <v>26.96671983207558</v>
+        <v>27.42957274064982</v>
       </c>
       <c r="F33" t="n">
-        <v>-56.19389083404489</v>
+        <v>-70.25849805662929</v>
       </c>
       <c r="G33" t="n">
-        <v>-35939859.89</v>
+        <v>-32989526.47</v>
       </c>
       <c r="H33" t="n">
-        <v>9.07918669424096</v>
+        <v>8.333868598610552</v>
       </c>
       <c r="I33" t="n">
-        <v>639568.8100000001</v>
+        <v>469545</v>
       </c>
       <c r="J33" t="n">
-        <v>4.913447744149143</v>
+        <v>3.607250361421642</v>
       </c>
       <c r="K33" t="n">
-        <v>0.017795528751573</v>
+        <v>0.0142331536776375</v>
       </c>
     </row>
     <row r="34">
@@ -1486,34 +1486,34 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="C34" t="n">
-        <v>25.8578431372549</v>
+        <v>26.83823529411764</v>
       </c>
       <c r="D34" t="n">
         <v>22.36666666666905</v>
       </c>
       <c r="E34" t="n">
-        <v>27.50930897474008</v>
+        <v>27.68425856625442</v>
       </c>
       <c r="F34" t="n">
-        <v>18.17712731440906</v>
+        <v>17.3446718558346</v>
       </c>
       <c r="G34" t="n">
-        <v>58258823.66</v>
+        <v>57080696.74</v>
       </c>
       <c r="H34" t="n">
-        <v>-14.71744014069395</v>
+        <v>-14.41981977464552</v>
       </c>
       <c r="I34" t="n">
-        <v>3205062.2</v>
+        <v>3290964.35</v>
       </c>
       <c r="J34" t="n">
-        <v>24.62269171076008</v>
+        <v>25.28262965416145</v>
       </c>
       <c r="K34" t="n">
-        <v>0.05501419353581229</v>
+        <v>0.05765459319794561</v>
       </c>
     </row>
     <row r="35">
@@ -1560,34 +1560,34 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C36" t="n">
-        <v>5.514705882352941</v>
+        <v>4.534313725490196</v>
       </c>
       <c r="D36" t="n">
         <v>21.33333333333666</v>
       </c>
       <c r="E36" t="n">
-        <v>27.01045950175392</v>
+        <v>25.57539841488741</v>
       </c>
       <c r="F36" t="n">
-        <v>-7.776253663990573</v>
+        <v>-6.667715829517041</v>
       </c>
       <c r="G36" t="n">
-        <v>-4246494.859999999</v>
+        <v>-3068367.94</v>
       </c>
       <c r="H36" t="n">
-        <v>1.072756536838982</v>
+        <v>0.7751361707905517</v>
       </c>
       <c r="I36" t="n">
-        <v>546084.92</v>
+        <v>460182.77</v>
       </c>
       <c r="J36" t="n">
-        <v>4.195263553092692</v>
+        <v>3.535325609691323</v>
       </c>
       <c r="K36" t="n">
-        <v>0.1285966280434872</v>
+        <v>0.1499763975502886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added volume_weighted_avg_spread_in_USD to pivots_CI_test
</commit_message>
<xml_diff>
--- a/processed_CI_test_data/pivots_CI_test.xlsx
+++ b/processed_CI_test_data/pivots_CI_test.xlsx
@@ -417,25 +417,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="27" customWidth="1" min="3" max="3"/>
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="33" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="35" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="31" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="9" max="9"/>
+    <col width="19" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="31" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,30 +469,35 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -511,34 +517,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C4" t="n">
-        <v>27.25060827250608</v>
+        <v>26.71394799054373</v>
       </c>
       <c r="D4" t="n">
-        <v>9.238095238093175</v>
+        <v>9.083333333331161</v>
       </c>
       <c r="E4" t="n">
-        <v>8.852830114165277</v>
+        <v>8.800082670593104</v>
       </c>
       <c r="F4" t="n">
-        <v>-6.481880931716827</v>
+        <v>7.145760355215238</v>
       </c>
       <c r="G4" t="n">
-        <v>-23579322.61</v>
+        <v>-7.246439295241086</v>
       </c>
       <c r="H4" t="n">
-        <v>21.57057258119731</v>
+        <v>-26774974.35</v>
       </c>
       <c r="I4" t="n">
-        <v>3637728.44</v>
+        <v>23.97303753726283</v>
       </c>
       <c r="J4" t="n">
-        <v>29.35136735063917</v>
+        <v>3694914.6</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1542762063256744</v>
+        <v>28.9410265661055</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.1379988100716892</v>
       </c>
     </row>
     <row r="5">
@@ -548,34 +557,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C5" t="n">
-        <v>22.01946472019465</v>
+        <v>21.27659574468085</v>
       </c>
       <c r="D5" t="n">
-        <v>9.071428571428919</v>
+        <v>9.093750000000247</v>
       </c>
       <c r="E5" t="n">
-        <v>8.86126499577688</v>
+        <v>8.767938246146342</v>
       </c>
       <c r="F5" t="n">
-        <v>-24.8523851949431</v>
+        <v>7.593880954716576</v>
       </c>
       <c r="G5" t="n">
-        <v>-71957539.43000001</v>
+        <v>-23.39170510734847</v>
       </c>
       <c r="H5" t="n">
-        <v>65.8273926147865</v>
+        <v>-71235880.26000001</v>
       </c>
       <c r="I5" t="n">
-        <v>2895397.72</v>
+        <v>63.78121633841791</v>
       </c>
       <c r="J5" t="n">
-        <v>23.36179940521428</v>
+        <v>3045347.91</v>
       </c>
       <c r="K5" t="n">
-        <v>0.04023758653972084</v>
+        <v>23.85318858691453</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.04275019693565867</v>
       </c>
     </row>
     <row r="6">
@@ -585,34 +597,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C6" t="n">
-        <v>8.759124087591241</v>
+        <v>8.747044917257684</v>
       </c>
       <c r="D6" t="n">
-        <v>9.187499999998433</v>
+        <v>9.52631578947196</v>
       </c>
       <c r="E6" t="n">
-        <v>8.778132596956828</v>
+        <v>9.379946294170733</v>
       </c>
       <c r="F6" t="n">
-        <v>-7.949343487081481</v>
+        <v>6.577107975926827</v>
       </c>
       <c r="G6" t="n">
-        <v>-10028895.4</v>
+        <v>-7.069095899808215</v>
       </c>
       <c r="H6" t="n">
-        <v>9.174522089247407</v>
+        <v>-7893483.26</v>
       </c>
       <c r="I6" t="n">
-        <v>1261600.46</v>
+        <v>7.067449179152464</v>
       </c>
       <c r="J6" t="n">
-        <v>10.17934657904133</v>
+        <v>1116618.5</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1257965518316204</v>
+        <v>8.746098129765944</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.1414608054796838</v>
       </c>
     </row>
     <row r="7">
@@ -622,34 +637,37 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C7" t="n">
-        <v>21.04622871046229</v>
+        <v>19.50354609929078</v>
       </c>
       <c r="D7" t="n">
-        <v>11.96774193548222</v>
+        <v>11.08695652173802</v>
       </c>
       <c r="E7" t="n">
-        <v>8.900441625092496</v>
+        <v>9.446417343921874</v>
       </c>
       <c r="F7" t="n">
-        <v>2.885413266690517</v>
+        <v>7.565519420988649</v>
       </c>
       <c r="G7" t="n">
-        <v>6686267.26</v>
+        <v>1.520985848618986</v>
       </c>
       <c r="H7" t="n">
-        <v>-6.116656343976</v>
+        <v>3384124.43</v>
       </c>
       <c r="I7" t="n">
-        <v>2317265.03</v>
+        <v>-3.029983929420951</v>
       </c>
       <c r="J7" t="n">
-        <v>18.69707930818494</v>
+        <v>2224954.58</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3465708054870663</v>
+        <v>17.4273228420917</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.6574683130076278</v>
       </c>
     </row>
     <row r="8">
@@ -659,34 +677,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C8" t="n">
-        <v>12.1654501216545</v>
+        <v>13.35697399527187</v>
       </c>
       <c r="D8" t="n">
-        <v>8.076923076924372</v>
+        <v>8.437500000000846</v>
       </c>
       <c r="E8" t="n">
-        <v>8.645833435275494</v>
+        <v>8.534704789202021</v>
       </c>
       <c r="F8" t="n">
-        <v>-5.994532945326227</v>
+        <v>7.444681455572622</v>
       </c>
       <c r="G8" t="n">
-        <v>-7787332.48</v>
+        <v>-5.534657292106162</v>
       </c>
       <c r="H8" t="n">
-        <v>7.123920532073131</v>
+        <v>-8592906.619999999</v>
       </c>
       <c r="I8" t="n">
-        <v>1299072.43</v>
+        <v>7.693679562963027</v>
       </c>
       <c r="J8" t="n">
-        <v>10.48169283027006</v>
+        <v>1552563.45</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1668186677962413</v>
+        <v>12.16070868106516</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.1806796604057592</v>
       </c>
     </row>
     <row r="9">
@@ -696,34 +717,37 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C9" t="n">
-        <v>8.759124087591241</v>
+        <v>10.40189125295508</v>
       </c>
       <c r="D9" t="n">
-        <v>10.91666666666317</v>
+        <v>11.99999999999634</v>
       </c>
       <c r="E9" t="n">
-        <v>9.881276003455296</v>
+        <v>10.43757810051786</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.692308960446939</v>
+        <v>7.010237214750169</v>
       </c>
       <c r="G9" t="n">
-        <v>-2645633.1</v>
+        <v>-0.5074365661726118</v>
       </c>
       <c r="H9" t="n">
-        <v>2.420248526671651</v>
+        <v>-574747.2299999999</v>
       </c>
       <c r="I9" t="n">
-        <v>982663.26</v>
+        <v>0.5146013116247049</v>
       </c>
       <c r="J9" t="n">
-        <v>7.928714526650221</v>
+        <v>1132648.43</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3714283964771986</v>
+        <v>8.871655194057174</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.97068967170142</v>
       </c>
     </row>
     <row r="10">
@@ -756,30 +780,35 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -799,34 +828,37 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="C13" t="n">
-        <v>26.88564476885645</v>
+        <v>22.93144208037825</v>
       </c>
       <c r="D13" t="n">
-        <v>9.65217391304312</v>
+        <v>9.53846153846129</v>
       </c>
       <c r="E13" t="n">
-        <v>12.06569886518193</v>
+        <v>12.13233169369355</v>
       </c>
       <c r="F13" t="n">
-        <v>-3.331625868918142</v>
+        <v>10.16730385952625</v>
       </c>
       <c r="G13" t="n">
-        <v>-6595114.591583</v>
+        <v>-5.397910605132456</v>
       </c>
       <c r="H13" t="n">
-        <v>6.826952680458853</v>
+        <v>-9331144.373677</v>
       </c>
       <c r="I13" t="n">
-        <v>1979548.38</v>
+        <v>9.728966156194963</v>
       </c>
       <c r="J13" t="n">
-        <v>26.3784536249036</v>
+        <v>1728658.56</v>
       </c>
       <c r="K13" t="n">
-        <v>0.3001537505544474</v>
+        <v>22.10888035498022</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.1852568656933995</v>
       </c>
     </row>
     <row r="14">
@@ -836,34 +868,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C14" t="n">
-        <v>17.51824817518248</v>
+        <v>17.49408983451537</v>
       </c>
       <c r="D14" t="n">
-        <v>11.94285714285589</v>
+        <v>12.03225806451507</v>
       </c>
       <c r="E14" t="n">
-        <v>12.55108358265023</v>
+        <v>12.57051141266667</v>
       </c>
       <c r="F14" t="n">
-        <v>-43.24430559978194</v>
+        <v>10.58948804115388</v>
       </c>
       <c r="G14" t="n">
-        <v>-55570122.7790099</v>
+        <v>-41.03899665831257</v>
       </c>
       <c r="H14" t="n">
-        <v>57.52357952108448</v>
+        <v>-52182367.9508599</v>
       </c>
       <c r="I14" t="n">
-        <v>1285027.52</v>
+        <v>54.40709857369549</v>
       </c>
       <c r="J14" t="n">
-        <v>17.12362232998058</v>
+        <v>1271531.28</v>
       </c>
       <c r="K14" t="n">
-        <v>0.02312443190219807</v>
+        <v>16.26239766928574</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.02436706745844497</v>
       </c>
     </row>
     <row r="15">
@@ -873,34 +908,37 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="C15" t="n">
-        <v>12.04379562043796</v>
+        <v>14.65721040189125</v>
       </c>
       <c r="D15" t="n">
-        <v>11.2285714285689</v>
+        <v>11.12765957446561</v>
       </c>
       <c r="E15" t="n">
-        <v>11.97877220222749</v>
+        <v>11.9964327658</v>
       </c>
       <c r="F15" t="n">
-        <v>-7.884856609133799</v>
+        <v>9.790757268098226</v>
       </c>
       <c r="G15" t="n">
-        <v>-7930868.6898764</v>
+        <v>-7.823823050719136</v>
       </c>
       <c r="H15" t="n">
-        <v>8.209662547762191</v>
+        <v>-10358295.1353324</v>
       </c>
       <c r="I15" t="n">
-        <v>1005835.5</v>
+        <v>10.79990821831177</v>
       </c>
       <c r="J15" t="n">
-        <v>13.40325165027375</v>
+        <v>1323942.92</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1268253881550113</v>
+        <v>16.93272245451591</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.1278147516268385</v>
       </c>
     </row>
     <row r="16">
@@ -910,34 +948,37 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C16" t="n">
-        <v>24.69586374695864</v>
+        <v>23.75886524822695</v>
       </c>
       <c r="D16" t="n">
-        <v>12.31249999999892</v>
+        <v>12.55555555555693</v>
       </c>
       <c r="E16" t="n">
-        <v>13.64131375263973</v>
+        <v>14.03384689476582</v>
       </c>
       <c r="F16" t="n">
-        <v>2.028021361045344</v>
+        <v>11.27023592750013</v>
       </c>
       <c r="G16" t="n">
-        <v>3630665.201051</v>
+        <v>3.751553558781449</v>
       </c>
       <c r="H16" t="n">
-        <v>-3.758293988977442</v>
+        <v>6683405.68286</v>
       </c>
       <c r="I16" t="n">
-        <v>1790249.98</v>
+        <v>-6.968344405868774</v>
       </c>
       <c r="J16" t="n">
-        <v>23.8559595469016</v>
+        <v>1781503.47</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4930914531810206</v>
+        <v>22.78474649742982</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.2665562371245507</v>
       </c>
     </row>
     <row r="17">
@@ -947,34 +988,37 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C17" t="n">
-        <v>5.109489051094891</v>
+        <v>6.501182033096926</v>
       </c>
       <c r="D17" t="n">
         <v>10.6666666666663</v>
       </c>
       <c r="E17" t="n">
-        <v>15.50636992327898</v>
+        <v>15.26724701789474</v>
       </c>
       <c r="F17" t="n">
-        <v>-49.05833341264378</v>
+        <v>11.25885038668071</v>
       </c>
       <c r="G17" t="n">
-        <v>-18661976.94242</v>
+        <v>-44.44149006024582</v>
       </c>
       <c r="H17" t="n">
-        <v>19.31800149042371</v>
+        <v>-21707835.12738</v>
       </c>
       <c r="I17" t="n">
-        <v>380403.81</v>
+        <v>22.63332179001721</v>
       </c>
       <c r="J17" t="n">
-        <v>5.069067451042363</v>
+        <v>488458.76</v>
       </c>
       <c r="K17" t="n">
-        <v>0.02038389668863619</v>
+        <v>6.247200304947436</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.02250149575642894</v>
       </c>
     </row>
     <row r="18">
@@ -984,34 +1028,37 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="C18" t="n">
-        <v>13.74695863746959</v>
+        <v>14.65721040189125</v>
       </c>
       <c r="D18" t="n">
-        <v>14.63157894736813</v>
+        <v>13.92307692307557</v>
       </c>
       <c r="E18" t="n">
-        <v>13.18686120617628</v>
+        <v>13.25599805002062</v>
       </c>
       <c r="F18" t="n">
-        <v>-10.79293837831121</v>
+        <v>11.68507421398226</v>
       </c>
       <c r="G18" t="n">
-        <v>-11476658.72062747</v>
+        <v>-7.360470106054805</v>
       </c>
       <c r="H18" t="n">
-        <v>11.8800977492482</v>
+        <v>-9014718.318076471</v>
       </c>
       <c r="I18" t="n">
-        <v>1063348.86</v>
+        <v>9.399049667649333</v>
       </c>
       <c r="J18" t="n">
-        <v>14.16964539689811</v>
+        <v>1224747.63</v>
       </c>
       <c r="K18" t="n">
-        <v>0.09265317422820978</v>
+        <v>15.66405271884089</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.1358608873606305</v>
       </c>
     </row>
     <row r="19">
@@ -1044,30 +1091,35 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -1087,34 +1139,37 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C22" t="n">
-        <v>28.71046228710462</v>
+        <v>26.47754137115839</v>
       </c>
       <c r="D22" t="n">
-        <v>13.1463414634122</v>
+        <v>13.1851851851844</v>
       </c>
       <c r="E22" t="n">
-        <v>10.07494494250078</v>
+        <v>10.34685395133333</v>
       </c>
       <c r="F22" t="n">
-        <v>-12.38068396427622</v>
+        <v>9.163127877642182</v>
       </c>
       <c r="G22" t="n">
-        <v>-9540380</v>
+        <v>-13.18924566073865</v>
       </c>
       <c r="H22" t="n">
-        <v>21.77379575107919</v>
+        <v>-10835274.73</v>
       </c>
       <c r="I22" t="n">
-        <v>770585.86</v>
+        <v>24.12401358546816</v>
       </c>
       <c r="J22" t="n">
-        <v>31.07681385656754</v>
+        <v>821523.46</v>
       </c>
       <c r="K22" t="n">
-        <v>0.08077098186864674</v>
+        <v>31.51593716196982</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.07581934749890738</v>
       </c>
     </row>
     <row r="23">
@@ -1124,34 +1179,37 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C23" t="n">
-        <v>22.26277372262774</v>
+        <v>22.10401891252955</v>
       </c>
       <c r="D23" t="n">
-        <v>13.51162790697708</v>
+        <v>13.88461538461494</v>
       </c>
       <c r="E23" t="n">
-        <v>9.988673944203958</v>
+        <v>10.04526055128462</v>
       </c>
       <c r="F23" t="n">
-        <v>-34.70745470820438</v>
+        <v>9.149045741219078</v>
       </c>
       <c r="G23" t="n">
-        <v>-27500391</v>
+        <v>-35.88564209826237</v>
       </c>
       <c r="H23" t="n">
-        <v>62.76352689398289</v>
+        <v>-27103837.67</v>
       </c>
       <c r="I23" t="n">
-        <v>792348.25</v>
+        <v>60.34487952197994</v>
       </c>
       <c r="J23" t="n">
-        <v>31.95446523613481</v>
+        <v>755283.62</v>
       </c>
       <c r="K23" t="n">
-        <v>0.02881225397849798</v>
+        <v>28.97479167227323</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.02786629809386694</v>
       </c>
     </row>
     <row r="24">
@@ -1161,34 +1219,37 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C24" t="n">
-        <v>9.732360097323602</v>
+        <v>11.93853427895981</v>
       </c>
       <c r="D24" t="n">
-        <v>12.11999999999755</v>
+        <v>12.06896551723818</v>
       </c>
       <c r="E24" t="n">
-        <v>10.75513796568648</v>
+        <v>10.55060927626582</v>
       </c>
       <c r="F24" t="n">
-        <v>-11.89809917186085</v>
+        <v>10.22009300772916</v>
       </c>
       <c r="G24" t="n">
-        <v>-3421235</v>
+        <v>-9.084252122986966</v>
       </c>
       <c r="H24" t="n">
-        <v>7.808208069955644</v>
+        <v>-3171260</v>
       </c>
       <c r="I24" t="n">
-        <v>287544.67</v>
+        <v>7.060598021685028</v>
       </c>
       <c r="J24" t="n">
-        <v>11.59633552715091</v>
+        <v>349094.23</v>
       </c>
       <c r="K24" t="n">
-        <v>0.08404703856940549</v>
+        <v>13.39223083938009</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.1100806083386414</v>
       </c>
     </row>
     <row r="25">
@@ -1198,34 +1259,37 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C25" t="n">
-        <v>19.4647201946472</v>
+        <v>19.62174940898345</v>
       </c>
       <c r="D25" t="n">
-        <v>13.55555555555233</v>
+        <v>13.81818181817928</v>
       </c>
       <c r="E25" t="n">
-        <v>10.00578773567213</v>
+        <v>10.30664709236364</v>
       </c>
       <c r="F25" t="n">
-        <v>-3.652974311016731</v>
+        <v>8.111806541144686</v>
       </c>
       <c r="G25" t="n">
-        <v>-1034127</v>
+        <v>-4.468655591029096</v>
       </c>
       <c r="H25" t="n">
-        <v>2.36016490733873</v>
+        <v>-1399487.57</v>
       </c>
       <c r="I25" t="n">
-        <v>283091.78</v>
+        <v>3.115865355762311</v>
       </c>
       <c r="J25" t="n">
-        <v>11.41675575436119</v>
+        <v>313178.66</v>
       </c>
       <c r="K25" t="n">
-        <v>0.2737495297966304</v>
+        <v>12.01440914302059</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.2237809514806909</v>
       </c>
     </row>
     <row r="26">
@@ -1235,34 +1299,37 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C26" t="n">
-        <v>9.732360097323602</v>
+        <v>8.392434988179669</v>
       </c>
       <c r="D26" t="n">
-        <v>14.09999999999906</v>
+        <v>15.2500000000017</v>
       </c>
       <c r="E26" t="n">
-        <v>10.68340684987277</v>
+        <v>12.00305448664</v>
       </c>
       <c r="F26" t="n">
-        <v>-11.44721215771162</v>
+        <v>8.342440709459956</v>
       </c>
       <c r="G26" t="n">
-        <v>-1932510</v>
+        <v>-13.16094076206549</v>
       </c>
       <c r="H26" t="n">
-        <v>4.410524321559314</v>
+        <v>-1848576.79</v>
       </c>
       <c r="I26" t="n">
-        <v>168819.27</v>
+        <v>4.115732430140342</v>
       </c>
       <c r="J26" t="n">
-        <v>6.808280947682607</v>
+        <v>140459.32</v>
       </c>
       <c r="K26" t="n">
-        <v>0.08735751432075384</v>
+        <v>5.388412283360735</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.0759824102303048</v>
       </c>
     </row>
     <row r="27">
@@ -1272,34 +1339,37 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C27" t="n">
-        <v>10.09732360097324</v>
+        <v>11.46572104018913</v>
       </c>
       <c r="D27" t="n">
-        <v>15.41176470588232</v>
+        <v>14.94999999999886</v>
       </c>
       <c r="E27" t="n">
-        <v>10.69812942788872</v>
+        <v>10.633229949</v>
       </c>
       <c r="F27" t="n">
-        <v>-2.184973665107742</v>
+        <v>9.379553441179803</v>
       </c>
       <c r="G27" t="n">
-        <v>-387236</v>
+        <v>-2.449696561161502</v>
       </c>
       <c r="H27" t="n">
-        <v>0.8837800560842337</v>
+        <v>-556455.58</v>
       </c>
       <c r="I27" t="n">
-        <v>177226.85</v>
+        <v>1.238911084964208</v>
       </c>
       <c r="J27" t="n">
-        <v>7.147348678102941</v>
+        <v>227152.86</v>
       </c>
       <c r="K27" t="n">
-        <v>0.4576714200126021</v>
+        <v>8.714218899995537</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.408213823644288</v>
       </c>
     </row>
     <row r="28">
@@ -1332,30 +1402,35 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>volume_weighted_avg_spread_in_USD</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>PnL_per_lot</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>total_profit</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>pct_total_profit</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>total_volume</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>pct_total_volume</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>pct_impact_on_PnL_exec_spread</t>
         </is>
@@ -1375,34 +1450,37 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="C31" t="n">
-        <v>26.10294117647059</v>
+        <v>27.9236276849642</v>
       </c>
       <c r="D31" t="n">
-        <v>20.26530612245328</v>
+        <v>20.76595744681236</v>
       </c>
       <c r="E31" t="n">
-        <v>27.11394847784483</v>
+        <v>27.35697571637037</v>
       </c>
       <c r="F31" t="n">
-        <v>-43.83208611641295</v>
+        <v>24.5843936986288</v>
       </c>
       <c r="G31" t="n">
-        <v>-167242396.71</v>
+        <v>-46.45713917658892</v>
       </c>
       <c r="H31" t="n">
-        <v>42.2490501512748</v>
+        <v>-166668754.47</v>
       </c>
       <c r="I31" t="n">
-        <v>3815524.46</v>
+        <v>38.23268832562583</v>
       </c>
       <c r="J31" t="n">
-        <v>29.31253018847632</v>
+        <v>3587581.1</v>
       </c>
       <c r="K31" t="n">
-        <v>0.022814337363367</v>
+        <v>26.45322861051847</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.02152521695748171</v>
       </c>
     </row>
     <row r="32">
@@ -1415,31 +1493,34 @@
         <v>161</v>
       </c>
       <c r="C32" t="n">
-        <v>19.73039215686275</v>
+        <v>19.21241050119332</v>
       </c>
       <c r="D32" t="n">
-        <v>22.00000000000272</v>
+        <v>21.12000000000353</v>
       </c>
       <c r="E32" t="n">
-        <v>31.22843153028255</v>
+        <v>30.79435795365854</v>
       </c>
       <c r="F32" t="n">
-        <v>-89.40773467472627</v>
+        <v>29.11358610980235</v>
       </c>
       <c r="G32" t="n">
-        <v>-243845293.77</v>
+        <v>-86.50893674627886</v>
       </c>
       <c r="H32" t="n">
-        <v>61.60060037590372</v>
+        <v>-273422756.32</v>
       </c>
       <c r="I32" t="n">
-        <v>2727340.03</v>
+        <v>62.72133644220483</v>
       </c>
       <c r="J32" t="n">
-        <v>20.95262074761143</v>
+        <v>3160630.18</v>
       </c>
       <c r="K32" t="n">
-        <v>0.01118471465179264</v>
+        <v>23.30508227530915</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.01155949937210406</v>
       </c>
     </row>
     <row r="33">
@@ -1449,34 +1530,37 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C33" t="n">
-        <v>7.107843137254902</v>
+        <v>7.040572792362769</v>
       </c>
       <c r="D33" t="n">
-        <v>21.40000000000327</v>
+        <v>20.6666666666706</v>
       </c>
       <c r="E33" t="n">
-        <v>27.24999773703315</v>
+        <v>26.53536187878788</v>
       </c>
       <c r="F33" t="n">
-        <v>-54.35968343221394</v>
+        <v>23.96186508307103</v>
       </c>
       <c r="G33" t="n">
-        <v>-33232703.86</v>
+        <v>-44.66863611574848</v>
       </c>
       <c r="H33" t="n">
-        <v>8.395300472034258</v>
+        <v>-39888229.5</v>
       </c>
       <c r="I33" t="n">
-        <v>611348.37</v>
+        <v>9.150090856466061</v>
       </c>
       <c r="J33" t="n">
-        <v>4.696645962872634</v>
+        <v>892980.6900000001</v>
       </c>
       <c r="K33" t="n">
-        <v>0.01839598645284591</v>
+        <v>6.584442742590131</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.02238707260747184</v>
       </c>
     </row>
     <row r="34">
@@ -1486,34 +1570,37 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C34" t="n">
-        <v>26.22549019607843</v>
+        <v>25.77565632458234</v>
       </c>
       <c r="D34" t="n">
-        <v>22.12500000000261</v>
+        <v>21.94444444444722</v>
       </c>
       <c r="E34" t="n">
-        <v>27.29314777456975</v>
+        <v>27.31399779281879</v>
       </c>
       <c r="F34" t="n">
-        <v>18.43937797983389</v>
+        <v>24.87698885614075</v>
       </c>
       <c r="G34" t="n">
-        <v>60130071.62</v>
+        <v>15.08552082243324</v>
       </c>
       <c r="H34" t="n">
-        <v>-15.19015788728663</v>
+        <v>47854004.64</v>
       </c>
       <c r="I34" t="n">
-        <v>3260959.87</v>
+        <v>-10.9773859554671</v>
       </c>
       <c r="J34" t="n">
-        <v>25.05212209615472</v>
+        <v>3172181.14</v>
       </c>
       <c r="K34" t="n">
-        <v>0.05423176427608586</v>
+        <v>23.39025392078107</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.06628872889247081</v>
       </c>
     </row>
     <row r="35">
@@ -1523,34 +1610,37 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C35" t="n">
-        <v>14.95098039215686</v>
+        <v>14.43914081145585</v>
       </c>
       <c r="D35" t="n">
-        <v>21.93548387097053</v>
+        <v>22.17857142857399</v>
       </c>
       <c r="E35" t="n">
-        <v>29.47713841592064</v>
+        <v>29.43266380088235</v>
       </c>
       <c r="F35" t="n">
-        <v>-3.790815904769366</v>
+        <v>27.73715359764924</v>
       </c>
       <c r="G35" t="n">
-        <v>-7614171.87</v>
+        <v>-1.267282281380241</v>
       </c>
       <c r="H35" t="n">
-        <v>1.923504658653465</v>
+        <v>-2514695.109999999</v>
       </c>
       <c r="I35" t="n">
-        <v>2008583.92</v>
+        <v>0.5768541001001538</v>
       </c>
       <c r="J35" t="n">
-        <v>15.43082147901841</v>
+        <v>1984321.21</v>
       </c>
       <c r="K35" t="n">
-        <v>0.263795453306467</v>
+        <v>14.63150271497155</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.789090177218343</v>
       </c>
     </row>
     <row r="36">
@@ -1560,34 +1650,37 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="n">
-        <v>5.88235294117647</v>
+        <v>5.608591885441527</v>
       </c>
       <c r="D36" t="n">
         <v>21.50000000000318</v>
       </c>
       <c r="E36" t="n">
-        <v>26.94284840873962</v>
+        <v>26.96942886</v>
       </c>
       <c r="F36" t="n">
-        <v>-6.820869092440554</v>
+        <v>25.67835588685672</v>
       </c>
       <c r="G36" t="n">
-        <v>-4044396.95</v>
+        <v>-1.690700297241644</v>
       </c>
       <c r="H36" t="n">
-        <v>1.021702229420369</v>
+        <v>-1292175</v>
       </c>
       <c r="I36" t="n">
-        <v>592944.52</v>
+        <v>0.2964162310702217</v>
       </c>
       <c r="J36" t="n">
-        <v>4.555259525866491</v>
+        <v>764283.89</v>
       </c>
       <c r="K36" t="n">
-        <v>0.1466088831859098</v>
+        <v>5.635489735829623</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.5914708843616383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>